<commit_message>
report page fix city
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="WEEKLY MEAL DATA" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="MONTHLY MEAL DATA" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Employee ID</t>
   </si>
@@ -31,40 +31,25 @@
     <t>City</t>
   </si>
   <si>
-    <t>Jane Smith</t>
+    <t>John Doe</t>
   </si>
   <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>1:00 PM</t>
+    <t>3:49 PM</t>
   </si>
   <si>
     <t>15 July 2024</t>
   </si>
   <si>
-    <t>Islamabad</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>2:10 PM</t>
-  </si>
-  <si>
-    <t>Emily Davis</t>
-  </si>
-  <si>
-    <t>Diet</t>
-  </si>
-  <si>
-    <t>1:20 PM</t>
-  </si>
-  <si>
-    <t>Michael Brown</t>
-  </si>
-  <si>
-    <t>2:50 PM</t>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>4:02 PM</t>
+  </si>
+  <si>
+    <t>16 July 2024</t>
   </si>
 </sst>
 </file>
@@ -448,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -477,7 +462,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -500,58 +485,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AVL tree major fix
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>Employee ID</t>
   </si>
@@ -31,49 +31,58 @@
     <t>City</t>
   </si>
   <si>
-    <t>Emily Davis</t>
+    <t>Ava Martinez</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>2:30 PM</t>
+  </si>
+  <si>
+    <t>18 July 2024</t>
+  </si>
+  <si>
+    <t>Lahore</t>
+  </si>
+  <si>
+    <t>Hina Saeed</t>
+  </si>
+  <si>
+    <t>3:00 PM</t>
+  </si>
+  <si>
+    <t>17 July 2024</t>
+  </si>
+  <si>
+    <t>David Williams</t>
+  </si>
+  <si>
+    <t>1:30 PM</t>
+  </si>
+  <si>
+    <t>Sophia Wilson</t>
+  </si>
+  <si>
+    <t>2:00 PM</t>
+  </si>
+  <si>
+    <t>Fatima Yousaf</t>
+  </si>
+  <si>
+    <t>19 July 2024</t>
+  </si>
+  <si>
+    <t>Sana Abbas</t>
+  </si>
+  <si>
+    <t>15 July 2024</t>
+  </si>
+  <si>
+    <t>Ayesha Ahmed</t>
   </si>
   <si>
     <t>Diet</t>
-  </si>
-  <si>
-    <t>1:20 PM</t>
-  </si>
-  <si>
-    <t>15 July 2024</t>
-  </si>
-  <si>
-    <t>Islamabad</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>2:10 PM</t>
-  </si>
-  <si>
-    <t>6:38 PM</t>
-  </si>
-  <si>
-    <t>17 July 2024</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>1:00 PM</t>
-  </si>
-  <si>
-    <t>7:2 PM</t>
-  </si>
-  <si>
-    <t>Michael Brown</t>
-  </si>
-  <si>
-    <t>2:50 PM</t>
   </si>
 </sst>
 </file>
@@ -457,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -486,7 +495,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>56123</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -506,19 +515,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>18392</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -526,19 +535,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>16254</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -546,19 +555,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>21789</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -566,19 +575,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>23781</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -586,21 +595,101 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>74528</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>74528</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>74528</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>90432</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>90432</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
report page drastic changes
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Employee ID</t>
   </si>
@@ -29,54 +29,6 @@
   </si>
   <si>
     <t>City</t>
-  </si>
-  <si>
-    <t>Michael Johnson</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>1:40 PM</t>
-  </si>
-  <si>
-    <t>18 July 2024</t>
-  </si>
-  <si>
-    <t>Islamabad</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>11:29 AM</t>
-  </si>
-  <si>
-    <t>Noah Thompson</t>
-  </si>
-  <si>
-    <t>Mariam Khalid</t>
-  </si>
-  <si>
-    <t>1:10 PM</t>
-  </si>
-  <si>
-    <t>Ali Khan</t>
-  </si>
-  <si>
-    <t>Diet</t>
-  </si>
-  <si>
-    <t>2:10 PM</t>
-  </si>
-  <si>
-    <t>Noor Fatima</t>
-  </si>
-  <si>
-    <t>Omar Sheikh</t>
-  </si>
-  <si>
-    <t>2:40 PM</t>
   </si>
 </sst>
 </file>
@@ -460,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -487,166 +439,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>18790</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>28615</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>68273</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>73421</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>76341</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>76341</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>78901</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>98234</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
icons and time added.
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="DAILY MEAL DATA" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="MONTHLY MEAL DATA" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Employee ID</t>
   </si>
@@ -29,6 +29,39 @@
   </si>
   <si>
     <t>City</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>1:20 PM</t>
+  </si>
+  <si>
+    <t>1 July 2024</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>18 July 2024</t>
+  </si>
+  <si>
+    <t>Sara Malik</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>1:50 PM</t>
+  </si>
+  <si>
+    <t>2:20 PM</t>
+  </si>
+  <si>
+    <t>10 July 2024</t>
   </si>
 </sst>
 </file>
@@ -412,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -439,6 +472,106 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>28615</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>28615</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31489</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>28615</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>28615</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
feedback is now from backend
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="MONTHLY MEAL DATA" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="DAILY MEAL DATA" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Employee ID</t>
   </si>
@@ -31,79 +31,19 @@
     <t>City</t>
   </si>
   <si>
-    <t>Michael Johnson</t>
+    <t>David Williams</t>
   </si>
   <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>1:40 PM</t>
-  </si>
-  <si>
-    <t>1 July 2024</t>
+    <t>11:01 AM</t>
+  </si>
+  <si>
+    <t>31 July 2024</t>
   </si>
   <si>
     <t>Islamabad</t>
-  </si>
-  <si>
-    <t>Emma Brown</t>
-  </si>
-  <si>
-    <t>Diet</t>
-  </si>
-  <si>
-    <t>2:10 PM</t>
-  </si>
-  <si>
-    <t>2 July 2024</t>
-  </si>
-  <si>
-    <t>Sophia Williams</t>
-  </si>
-  <si>
-    <t>5 July 2024</t>
-  </si>
-  <si>
-    <t>Zara Iqbal</t>
-  </si>
-  <si>
-    <t>1:10 PM</t>
-  </si>
-  <si>
-    <t>8 July 2024</t>
-  </si>
-  <si>
-    <t>2:40 PM</t>
-  </si>
-  <si>
-    <t>11 July 2024</t>
-  </si>
-  <si>
-    <t>12 July 2024</t>
-  </si>
-  <si>
-    <t>14 July 2024</t>
-  </si>
-  <si>
-    <t>17 July 2024</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>12:53 PM</t>
-  </si>
-  <si>
-    <t>21 July 2024</t>
-  </si>
-  <si>
-    <t>Emily Davis</t>
-  </si>
-  <si>
-    <t>11:15 AM</t>
-  </si>
-  <si>
-    <t>22 July 2024</t>
   </si>
 </sst>
 </file>
@@ -487,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -516,7 +456,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18790</v>
+        <v>16254</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -531,186 +471,6 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>52837</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>35672</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>13487</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>18790</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>52837</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>35672</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>13487</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>28615</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>18264</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user added on enter press and fixed admin panel
</commit_message>
<xml_diff>
--- a/Backend/downloads/data.xlsx
+++ b/Backend/downloads/data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="DAILY MEAL DATA" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Feedbacks of 9 August 2024" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Employee ID</t>
   </si>
@@ -19,31 +19,46 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Meal Type</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>City</t>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>David Williams</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>11:01 AM</t>
-  </si>
-  <si>
-    <t>31 July 2024</t>
-  </si>
-  <si>
-    <t>Islamabad</t>
+    <t>HR Manager</t>
+  </si>
+  <si>
+    <t>Contour Software</t>
+  </si>
+  <si>
+    <t>This is good feedback</t>
+  </si>
+  <si>
+    <t>Sara Akbar</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>The food was really good today</t>
+  </si>
+  <si>
+    <t>Emma Brown</t>
+  </si>
+  <si>
+    <t>Autosoft</t>
+  </si>
+  <si>
+    <t>biryani was good.</t>
   </si>
 </sst>
 </file>
@@ -427,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -467,11 +482,51 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>28623</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>52837</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>